<commit_message>
question and answer model setting
</commit_message>
<xml_diff>
--- a/db_erd.xlsx
+++ b/db_erd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\web\business_blog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{113ACD4F-9D21-4609-9C75-38DB597C792B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11863B3F-F00E-4032-AE6A-8F08DAC44A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3555" yWindow="2085" windowWidth="21600" windowHeight="11385" xr2:uid="{8C2807C4-563D-45B3-80AB-A26016DB4F75}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="56">
   <si>
     <t>user</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -235,6 +235,30 @@
   </si>
   <si>
     <t>답변작성날짜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>notice(완료)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user(완료)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>modified_at</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수정날짜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>modifed_at</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>backref=notice_set</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -589,6 +613,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -598,30 +652,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -630,18 +660,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="36">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -861,23 +885,23 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
+        <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
@@ -895,6 +919,120 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -999,25 +1137,37 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -1034,42 +1184,56 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7D99033A-5E7E-4CC7-B679-32C9AC6DBC79}" name="표2" displayName="표2" ref="A2:E10" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="25" tableBorderDxfId="26" totalsRowBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7D99033A-5E7E-4CC7-B679-32C9AC6DBC79}" name="표2" displayName="표2" ref="A2:E10" totalsRowShown="0" headerRowDxfId="35" headerRowBorderDxfId="34" tableBorderDxfId="33" totalsRowBorderDxfId="32">
   <autoFilter ref="A2:E10" xr:uid="{7D99033A-5E7E-4CC7-B679-32C9AC6DBC79}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B2165067-7723-406E-9663-CFFAA49A24AD}" name="field" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{AAF79685-9FEB-4476-B972-2373B8F66EDC}" name="type" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{ECBAEB79-CEF2-4CF2-8A98-B8E369126E22}" name="content" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{10A09EFD-7341-4EB9-B890-9BEC48CA4F15}" name="null" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{8AF7C31B-B6F2-44D6-A2BB-30AE765C1B25}" name="constraint" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{B2165067-7723-406E-9663-CFFAA49A24AD}" name="field" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{AAF79685-9FEB-4476-B972-2373B8F66EDC}" name="type" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{ECBAEB79-CEF2-4CF2-8A98-B8E369126E22}" name="content" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{10A09EFD-7341-4EB9-B890-9BEC48CA4F15}" name="null" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{8AF7C31B-B6F2-44D6-A2BB-30AE765C1B25}" name="constraint" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{055F00CB-D8E4-4C3E-AF66-1027966AF60F}" name="표2_4" displayName="표2_4" ref="A16:E24" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="15" tableBorderDxfId="16" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{055F00CB-D8E4-4C3E-AF66-1027966AF60F}" name="표2_4" displayName="표2_4" ref="A16:E24" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="23">
   <autoFilter ref="A16:E24" xr:uid="{055F00CB-D8E4-4C3E-AF66-1027966AF60F}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{3B9FD2ED-6D30-4F5E-800E-25A58755577B}" name="field" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{893E0C3B-7CD1-465C-A7B7-4393BB91FD43}" name="type" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{AAFC0701-11C8-47DD-8099-24C46ED88030}" name="content" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{264BFC99-143B-4D09-A242-34521BA4CFD6}" name="null" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{22DA176B-7ECB-4A67-8CA0-49A5C3048774}" name="constraint" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{3B9FD2ED-6D30-4F5E-800E-25A58755577B}" name="field" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{893E0C3B-7CD1-465C-A7B7-4393BB91FD43}" name="type" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{AAFC0701-11C8-47DD-8099-24C46ED88030}" name="content" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{264BFC99-143B-4D09-A242-34521BA4CFD6}" name="null" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{22DA176B-7ECB-4A67-8CA0-49A5C3048774}" name="constraint" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D62F1A9A-31C0-415D-9A43-EFAB94667725}" name="표2_45" displayName="표2_45" ref="A30:E38" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D62F1A9A-31C0-415D-9A43-EFAB94667725}" name="표2_45" displayName="표2_45" ref="A30:E38" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="A30:E38" xr:uid="{D62F1A9A-31C0-415D-9A43-EFAB94667725}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{A154B91D-EA1E-42ED-B4E7-35C270E495A4}" name="field" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{75E6E491-53A5-4E74-AA1C-F689CCAB3D59}" name="type" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{B0B4AABE-E304-4CEA-8588-ED8AE2929D9C}" name="content" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{98FAB849-6FD0-4301-93EA-9F8F0B76C24E}" name="null" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{25F963E6-DF95-4DA1-8BFF-22B0E4A0ABB1}" name="constraint" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{A154B91D-EA1E-42ED-B4E7-35C270E495A4}" name="field" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{75E6E491-53A5-4E74-AA1C-F689CCAB3D59}" name="type" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{B0B4AABE-E304-4CEA-8588-ED8AE2929D9C}" name="content" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{98FAB849-6FD0-4301-93EA-9F8F0B76C24E}" name="null" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{25F963E6-DF95-4DA1-8BFF-22B0E4A0ABB1}" name="constraint" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5D9B47B5-5C4F-4184-823D-74F9D31EE5F3}" name="표2_42" displayName="표2_42" ref="A44:E52" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
+  <autoFilter ref="A44:E52" xr:uid="{5D9B47B5-5C4F-4184-823D-74F9D31EE5F3}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{2DFAC5E4-65CE-4986-9CD0-BCA219998E12}" name="field" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{B30A6DCC-9A21-479A-85E8-13920F0DBE7B}" name="type" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{41CDF5E1-C24D-43BE-A00E-3EEF9A9A57E3}" name="content" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{F173C648-4315-4E54-8F28-634E8B2DA7E7}" name="null" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{42C3BB6B-6FE6-47BB-B1AC-528CFE0FF0D7}" name="constraint" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1392,10 +1556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA5650EC-002F-45C9-91DA-860A3AE47109}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1408,33 +1572,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="9"/>
+      <c r="A1" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1443,15 +1607,15 @@
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="11" t="s">
+      <c r="D3" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1460,13 +1624,13 @@
       <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" s="11"/>
+      <c r="D4" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1475,15 +1639,15 @@
       <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="11" t="s">
+      <c r="D5" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1492,13 +1656,13 @@
       <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" s="11"/>
+      <c r="D6" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1507,15 +1671,15 @@
       <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="11" t="s">
+      <c r="D7" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1524,15 +1688,15 @@
       <c r="C8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" s="11" t="s">
+      <c r="D8" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1541,50 +1705,50 @@
       <c r="C9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" s="11"/>
+      <c r="D9" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" s="14"/>
+      <c r="D10" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="11"/>
     </row>
     <row r="14" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="20"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="22"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="22" t="s">
+      <c r="E16" s="16" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1598,7 +1762,7 @@
       <c r="C17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="11" t="b">
+      <c r="D17" s="8" t="b">
         <v>0</v>
       </c>
       <c r="E17" s="3" t="s">
@@ -1615,7 +1779,7 @@
       <c r="C18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="11" t="b">
+      <c r="D18" s="8" t="b">
         <v>0</v>
       </c>
       <c r="E18" s="3"/>
@@ -1630,7 +1794,7 @@
       <c r="C19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="11" t="b">
+      <c r="D19" s="8" t="b">
         <v>0</v>
       </c>
       <c r="E19" s="3"/>
@@ -1645,7 +1809,7 @@
       <c r="C20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="11" t="b">
+      <c r="D20" s="8" t="b">
         <v>0</v>
       </c>
       <c r="E20" s="3"/>
@@ -1660,7 +1824,7 @@
       <c r="C21" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="11" t="b">
+      <c r="D21" s="8" t="b">
         <v>0</v>
       </c>
       <c r="E21" s="3" t="s">
@@ -1677,7 +1841,7 @@
       <c r="C22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="11" t="b">
+      <c r="D22" s="8" t="b">
         <v>0</v>
       </c>
       <c r="E22" s="3" t="s">
@@ -1685,10 +1849,18 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="11"/>
+      <c r="A23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="8" t="b">
+        <v>0</v>
+      </c>
       <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1700,28 +1872,28 @@
     </row>
     <row r="28" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="20"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="22"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="21" t="s">
+      <c r="A30" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C30" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="17" t="s">
+      <c r="D30" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="22" t="s">
+      <c r="E30" s="16" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1735,7 +1907,7 @@
       <c r="C31" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D31" s="11" t="b">
+      <c r="D31" s="8" t="b">
         <v>0</v>
       </c>
       <c r="E31" s="3" t="s">
@@ -1750,7 +1922,7 @@
       <c r="C32" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="11" t="b">
+      <c r="D32" s="8" t="b">
         <v>0</v>
       </c>
       <c r="E32" s="3"/>
@@ -1763,7 +1935,7 @@
       <c r="C33" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D33" s="11" t="b">
+      <c r="D33" s="8" t="b">
         <v>0</v>
       </c>
       <c r="E33" s="3" t="s">
@@ -1778,7 +1950,7 @@
       <c r="C34" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="11" t="b">
+      <c r="D34" s="8" t="b">
         <v>0</v>
       </c>
       <c r="E34" s="3" t="s">
@@ -1793,7 +1965,7 @@
       <c r="C35" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="11" t="b">
+      <c r="D35" s="8" t="b">
         <v>0</v>
       </c>
       <c r="E35" s="3" t="s">
@@ -1808,7 +1980,7 @@
       <c r="C36" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D36" s="11" t="b">
+      <c r="D36" s="8" t="b">
         <v>0</v>
       </c>
       <c r="E36" s="3" t="s">
@@ -1825,7 +1997,7 @@
       <c r="C37" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D37" s="11" t="b">
+      <c r="D37" s="8" t="b">
         <v>0</v>
       </c>
       <c r="E37" s="3"/>
@@ -1837,18 +2009,165 @@
       <c r="D38" s="5"/>
       <c r="E38" s="6"/>
     </row>
+    <row r="42" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" s="21"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="22"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E44" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D45" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D46" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D47" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D48" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D49" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D50" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D51" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="4"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A15:E15"/>
     <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A43:E43"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="3">
+  <tableParts count="4">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>